<commit_message>
[ADD] Xl files to create iCZ843 barplots
</commit_message>
<xml_diff>
--- a/RdKit_Lipid_GEMA/final_results/iCZ843_H_xml.xlsx
+++ b/RdKit_Lipid_GEMA/final_results/iCZ843_H_xml.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
   <si>
     <t xml:space="preserve">Triacylglycerol</t>
   </si>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Phosphatidylglycerol</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Phosphatid</t>
+    <t xml:space="preserve">1-P-N-methylethanolamine</t>
   </si>
   <si>
     <t xml:space="preserve">Sulfoquinovosyldiacylglycerol</t>
@@ -133,25 +133,22 @@
     <t xml:space="preserve">2'-O-all-cis-5,9,12,15-octadecatetraenoyl-sulfoquinovosyldiacylglycerol (2'-//)</t>
   </si>
   <si>
-    <t xml:space="preserve">DG-Homoseri</t>
+    <t xml:space="preserve">DG-Homoserine</t>
   </si>
   <si>
     <t xml:space="preserve">1-Acyl-sn-glycero-3-phosphoethanolamine</t>
   </si>
   <si>
-    <t xml:space="preserve">2'-O-all-cis-5</t>
+    <t xml:space="preserve">Octadecatetraenoyl-SQDG</t>
   </si>
   <si>
     <t xml:space="preserve">1-monoacylglycerol</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Acyl-sn-gly</t>
+    <t xml:space="preserve">1-Acyl-sn-glycero-3-PE</t>
   </si>
   <si>
     <t xml:space="preserve">Palmitoyl-CoA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-monoacylgl</t>
   </si>
   <si>
     <t xml:space="preserve">2'-O-all-cis-5,9,12-octadecatrienoyl-sulfoquinovosyldiacylglycerol (2'-//)</t>
@@ -543,8 +540,8 @@
   </sheetPr>
   <dimension ref="A1:R292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1:R20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -557,10 +554,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="9.14"/>
   </cols>
   <sheetData>
@@ -1313,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M17" s="12" t="n">
         <v>0</v>
@@ -1336,7 +1333,7 @@
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>4</v>
@@ -1365,13 +1362,13 @@
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>4</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="M19" s="12" t="n">
         <v>0</v>
@@ -1394,7 +1391,7 @@
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>4</v>
@@ -1426,7 +1423,7 @@
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>3</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>2</v>
@@ -1445,7 +1442,7 @@
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>2</v>
@@ -1456,7 +1453,7 @@
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>2</v>
@@ -1465,7 +1462,7 @@
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>2</v>
@@ -1474,7 +1471,7 @@
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>2</v>
@@ -1482,7 +1479,7 @@
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>2</v>
@@ -1490,7 +1487,7 @@
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>2</v>
@@ -1498,7 +1495,7 @@
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>2</v>
@@ -1506,7 +1503,7 @@
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>2</v>
@@ -1514,7 +1511,7 @@
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>1</v>
@@ -1522,7 +1519,7 @@
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>1</v>
@@ -1530,7 +1527,7 @@
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>1</v>
@@ -1538,7 +1535,7 @@
     </row>
     <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>1</v>
@@ -1546,7 +1543,7 @@
     </row>
     <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>1</v>
@@ -1554,7 +1551,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>1</v>
@@ -1562,7 +1559,7 @@
     </row>
     <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>1</v>
@@ -1570,7 +1567,7 @@
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>1</v>
@@ -1578,7 +1575,7 @@
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>1</v>
@@ -1586,7 +1583,7 @@
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>1</v>
@@ -1594,7 +1591,7 @@
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="4" t="n">
         <v>1</v>
@@ -1602,7 +1599,7 @@
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="4" t="n">
         <v>1</v>
@@ -1610,7 +1607,7 @@
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="4" t="n">
         <v>1</v>
@@ -1618,7 +1615,7 @@
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="4" t="n">
         <v>1</v>
@@ -1626,7 +1623,7 @@
     </row>
     <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="4" t="n">
         <v>1</v>
@@ -1634,7 +1631,7 @@
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="4" t="n">
         <v>1</v>
@@ -1642,7 +1639,7 @@
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="4" t="n">
         <v>1</v>
@@ -1650,7 +1647,7 @@
     </row>
     <row r="48" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="4" t="n">
         <v>1</v>
@@ -1658,7 +1655,7 @@
     </row>
     <row r="49" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="4" t="n">
         <v>1</v>
@@ -1666,7 +1663,7 @@
     </row>
     <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="4" t="n">
         <v>1</v>
@@ -1674,7 +1671,7 @@
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4" t="n">
         <v>1</v>
@@ -1682,7 +1679,7 @@
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="4" t="n">
         <v>1</v>
@@ -1690,7 +1687,7 @@
     </row>
     <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="4" t="n">
         <v>1</v>
@@ -1698,7 +1695,7 @@
     </row>
     <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" s="4" t="n">
         <v>1</v>
@@ -1706,7 +1703,7 @@
     </row>
     <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="4" t="n">
         <v>1</v>

</xml_diff>